<commit_message>
FIX bug, when you edit book and try to add new one, fields weren't editable.
</commit_message>
<xml_diff>
--- a/management/Final Project Rubric (Vincent Picot and Hafsa Hussain).xlsx
+++ b/management/Final Project Rubric (Vincent Picot and Hafsa Hussain).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Documents/Classes/Second Semester/CSC 4992 - Python Programming/LibraryInventory/Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFB785E-7252-1147-B0CA-ED1629159DDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997E8922-7ABF-9544-A35C-E5B5F84F5FEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30060" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="75">
   <si>
     <t>Earned</t>
   </si>
@@ -700,6 +700,21 @@
   </si>
   <si>
     <t>Runs on my mac (MacBook pro 2016 15" touchbar), screenshots in the pdf file with this Excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hafsa Hussain </t>
+  </si>
+  <si>
+    <t>gh7070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hafsa-hussain </t>
+  </si>
+  <si>
+    <t>Windows 10</t>
+  </si>
+  <si>
+    <t>9A-5F-D3-39-9D-C8</t>
   </si>
 </sst>
 </file>
@@ -902,23 +917,23 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1238,8 +1253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C40D522-ECA1-FF4D-B661-39278A20B6C5}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1256,16 +1271,16 @@
   <sheetData>
     <row r="1" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="F1" s="29" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="F1" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -1320,19 +1335,19 @@
         <v>24</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="H5" s="21" t="s">
         <v>42</v>
@@ -1491,10 +1506,10 @@
       <c r="E16" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="G16" s="30" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1512,10 +1527,10 @@
       <c r="E17" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="32" t="s">
+      <c r="F17" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="G17" s="32" t="s">
+      <c r="G17" s="30" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1533,10 +1548,10 @@
       <c r="E18" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="30" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1554,10 +1569,10 @@
       <c r="E19" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="G19" s="30" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1575,10 +1590,10 @@
       <c r="E20" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="32" t="s">
+      <c r="F20" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="G20" s="32" t="s">
+      <c r="G20" s="30" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1596,10 +1611,10 @@
       <c r="E21" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="G21" s="32" t="s">
+      <c r="G21" s="30" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1617,10 +1632,10 @@
       <c r="E22" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="32" t="s">
+      <c r="F22" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="G22" s="30" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1638,10 +1653,10 @@
       <c r="E23" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="G23" s="34" t="s">
+      <c r="G23" s="32" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1659,10 +1674,10 @@
       <c r="E24" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="31" t="s">
+      <c r="F24" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="G24" s="31" t="s">
+      <c r="G24" s="29" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1680,10 +1695,10 @@
       <c r="E25" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F25" s="31" t="s">
+      <c r="F25" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="G25" s="31" t="s">
+      <c r="G25" s="29" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1737,12 +1752,12 @@
   <sheetData>
     <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:9" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="3"/>

</xml_diff>

<commit_message>
Upload management file (Final project report)
</commit_message>
<xml_diff>
--- a/management/Final Project Rubric (Vincent Picot and Hafsa Hussain).xlsx
+++ b/management/Final Project Rubric (Vincent Picot and Hafsa Hussain).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafsa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Documents/Classes/Second Semester/CSC 4992 - Python Programming/LibraryInventory/Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91C59A3-9139-475F-9FFC-649201DB5FBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC46FE74-7633-8848-A819-A82137AB8DA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13665" windowHeight="9728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="320" yWindow="920" windowWidth="29580" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group rubrik" sheetId="3" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -138,9 +139,6 @@
     <t>Student  _________________________</t>
   </si>
   <si>
-    <t>completed? Yes or not</t>
-  </si>
-  <si>
     <t xml:space="preserve">Name </t>
   </si>
   <si>
@@ -1211,6 +1209,9 @@
       </rPr>
       <t xml:space="preserve"> with bookSuggestions.txt. Asks user to input a book suggestion and writes it to a file using the append method each time a new book is added. The file is then read and has its contents printed out.</t>
     </r>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1749,111 +1750,111 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C40D522-ECA1-FF4D-B661-39278A20B6C5}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="59" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.33203125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="10.796875" style="2"/>
+    <col min="3" max="4" width="10.83203125" style="2"/>
     <col min="5" max="5" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="66.1328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="66.1640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="89.33203125" style="2" customWidth="1"/>
     <col min="8" max="9" width="32.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.796875" style="2"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="33"/>
       <c r="F1" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1" s="33"/>
       <c r="H1" s="33"/>
     </row>
-    <row r="2" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.85">
+    <row r="2" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="16"/>
     </row>
-    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.85">
+    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="16"/>
       <c r="C3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="19" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="E4" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="F4" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="G4" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="20" t="s">
-        <v>51</v>
-      </c>
       <c r="H4" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="E5" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="F5" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="G5" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="20" t="s">
-        <v>66</v>
-      </c>
       <c r="H5" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.85">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="16"/>
     </row>
-    <row r="7" spans="1:9" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:9" ht="24" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1871,7 +1872,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>21</v>
       </c>
@@ -1883,10 +1884,10 @@
         <v>2</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>21</v>
       </c>
@@ -1898,10 +1899,10 @@
         <v>2</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>21</v>
       </c>
@@ -1913,10 +1914,10 @@
         <v>2</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>21</v>
       </c>
@@ -1928,10 +1929,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>21</v>
       </c>
@@ -1943,10 +1944,10 @@
         <v>2</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>21</v>
       </c>
@@ -1958,17 +1959,17 @@
         <v>2</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="10"/>
       <c r="C14" s="23"/>
       <c r="D14" s="26"/>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
     </row>
-    <row r="15" spans="1:9" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="15" spans="1:9" ht="24" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
         <v>8</v>
       </c>
@@ -1982,13 +1983,13 @@
         <v>25</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>21</v>
       </c>
@@ -2003,13 +2004,13 @@
         <v>32</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G16" s="30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>21</v>
       </c>
@@ -2024,13 +2025,13 @@
         <v>32</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G17" s="30" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>21</v>
       </c>
@@ -2045,13 +2046,13 @@
         <v>32</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="85.05" customHeight="1" x14ac:dyDescent="0.45">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>21</v>
       </c>
@@ -2066,13 +2067,13 @@
         <v>32</v>
       </c>
       <c r="F19" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G19" s="30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="97.05" customHeight="1" x14ac:dyDescent="0.45">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="97" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>21</v>
       </c>
@@ -2087,13 +2088,13 @@
         <v>32</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="79.05" customHeight="1" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>21</v>
       </c>
@@ -2108,13 +2109,13 @@
         <v>32</v>
       </c>
       <c r="F21" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G21" s="30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="49.05" customHeight="1" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>21</v>
       </c>
@@ -2129,13 +2130,13 @@
         <v>32</v>
       </c>
       <c r="F22" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>21</v>
       </c>
@@ -2150,13 +2151,13 @@
         <v>32</v>
       </c>
       <c r="F23" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G23" s="32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="64.05" customHeight="1" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>21</v>
       </c>
@@ -2171,13 +2172,13 @@
         <v>27</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G24" s="29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>21</v>
       </c>
@@ -2192,17 +2193,17 @@
         <v>26</v>
       </c>
       <c r="F25" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G25" s="29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C26" s="23"/>
       <c r="D26" s="26"/>
     </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B27" s="13" t="s">
         <v>33</v>
       </c>
@@ -2237,17 +2238,17 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.33203125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="10.796875" style="2"/>
+    <col min="3" max="4" width="10.83203125" style="2"/>
     <col min="5" max="5" width="69.33203125" style="2" customWidth="1"/>
     <col min="6" max="9" width="32.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.796875" style="2"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="34" t="s">
         <v>34</v>
@@ -2256,7 +2257,7 @@
       <c r="D1" s="34"/>
       <c r="E1" s="34"/>
     </row>
-    <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:9" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
@@ -2266,7 +2267,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>21</v>
       </c>
@@ -2279,7 +2280,7 @@
       </c>
       <c r="E3" s="15"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>21</v>
       </c>
@@ -2292,7 +2293,7 @@
       </c>
       <c r="E4" s="15"/>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
@@ -2307,7 +2308,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>21</v>
       </c>
@@ -2320,7 +2321,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>21</v>
       </c>
@@ -2333,7 +2334,7 @@
       </c>
       <c r="E7" s="15"/>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="13" t="s">
         <v>20</v>
       </c>
@@ -2351,28 +2352,28 @@
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
     </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>

</xml_diff>